<commit_message>
Incorporacion Jenkinsfile desde Intellij Idea
</commit_message>
<xml_diff>
--- a/src/test/resources/filepath/Test2.xlsx
+++ b/src/test/resources/filepath/Test2.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="27">
   <si>
     <t>$ 27.323 CLP 17-10-20</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>$ 34.490 CLP 23-11-20</t>
+  </si>
+  <si>
+    <t>$ 27.553 CLP 26-11-20</t>
   </si>
 </sst>
 </file>
@@ -464,7 +467,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BFA8BFF-EFDD-4913-9E02-008959E8AF40}">
-  <dimension ref="A1:A91"/>
+  <dimension ref="A1:A92"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
@@ -930,6 +933,11 @@
         <v>24</v>
       </c>
     </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Run en CI teamcity
</commit_message>
<xml_diff>
--- a/src/test/resources/filepath/Test2.xlsx
+++ b/src/test/resources/filepath/Test2.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="33">
   <si>
     <t>$ 27.323 CLP 17-10-20</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>$ 34.696 CLP 10-02-21</t>
+  </si>
+  <si>
+    <t>0.95 UF 17-02-21</t>
   </si>
 </sst>
 </file>
@@ -482,7 +485,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BFA8BFF-EFDD-4913-9E02-008959E8AF40}">
-  <dimension ref="A1:A103"/>
+  <dimension ref="A1:A104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
@@ -1008,6 +1011,11 @@
         <v>31</v>
       </c>
     </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Agragando Replica de firefox
</commit_message>
<xml_diff>
--- a/src/test/resources/filepath/Test2.xlsx
+++ b/src/test/resources/filepath/Test2.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="34">
   <si>
     <t>$ 27.323 CLP 17-10-20</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>0.95 UF 17-02-21</t>
+  </si>
+  <si>
+    <t>0.95 UF 18-02-21</t>
   </si>
 </sst>
 </file>
@@ -485,7 +488,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BFA8BFF-EFDD-4913-9E02-008959E8AF40}">
-  <dimension ref="A1:A104"/>
+  <dimension ref="A1:A105"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
@@ -1016,6 +1019,11 @@
         <v>32</v>
       </c>
     </row>
+    <row r="105">
+      <c r="A105" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Agregando Escenario HomePageLogin Run en Edge
</commit_message>
<xml_diff>
--- a/src/test/resources/filepath/Test2.xlsx
+++ b/src/test/resources/filepath/Test2.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="70">
   <si>
     <t>$ 27.323 CLP 17-10-20</t>
   </si>
@@ -136,6 +136,114 @@
   </si>
   <si>
     <t>0.95 UF 18-02-21</t>
+  </si>
+  <si>
+    <t>0.95 UF 25-02-21</t>
+  </si>
+  <si>
+    <t>0.95 UF 02-03-21</t>
+  </si>
+  <si>
+    <t>$ 34.594 CLP 02-03-21</t>
+  </si>
+  <si>
+    <t>3.57 UF 03-03-21</t>
+  </si>
+  <si>
+    <t>0.95 UF 03-03-21</t>
+  </si>
+  <si>
+    <t>$ 34.594 CLP 04-03-21</t>
+  </si>
+  <si>
+    <t>3.57 UF 04-03-21</t>
+  </si>
+  <si>
+    <t>5.95 UF 04-03-21</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 04-03-21</t>
+  </si>
+  <si>
+    <t>23.80 UF 04-03-21</t>
+  </si>
+  <si>
+    <t>2.38 UF 04-03-21</t>
+  </si>
+  <si>
+    <t>7.14 UF 04-03-21</t>
+  </si>
+  <si>
+    <t>4.76 UF 04-03-21</t>
+  </si>
+  <si>
+    <t>13.09 UF 04-03-21</t>
+  </si>
+  <si>
+    <t>41.65 UF 04-03-21</t>
+  </si>
+  <si>
+    <t>22.61 UF 04-03-21</t>
+  </si>
+  <si>
+    <t>$ 69.187 CLP 04-03-21</t>
+  </si>
+  <si>
+    <t>$ 103.781 CLP 04-03-21</t>
+  </si>
+  <si>
+    <t>$ 172.968 CLP 04-03-21</t>
+  </si>
+  <si>
+    <t>$ 34.594 CLP 08-03-21</t>
+  </si>
+  <si>
+    <t>$ 69.187 CLP 08-03-21</t>
+  </si>
+  <si>
+    <t>3.57 UF 08-03-21</t>
+  </si>
+  <si>
+    <t>$ 103.781 CLP 08-03-21</t>
+  </si>
+  <si>
+    <t>5.95 UF 08-03-21</t>
+  </si>
+  <si>
+    <t>$ 172.968 CLP 08-03-21</t>
+  </si>
+  <si>
+    <t>23.80 UF 08-03-21</t>
+  </si>
+  <si>
+    <t>0.95 UF 08-03-21</t>
+  </si>
+  <si>
+    <t>2.38 UF 08-03-21</t>
+  </si>
+  <si>
+    <t>7.14 UF 08-03-21</t>
+  </si>
+  <si>
+    <t>4.76 UF 08-03-21</t>
+  </si>
+  <si>
+    <t>13.09 UF 08-03-21</t>
+  </si>
+  <si>
+    <t>41.65 UF 08-03-21</t>
+  </si>
+  <si>
+    <t>22.61 UF 08-03-21</t>
+  </si>
+  <si>
+    <t>41.65 UF 09-03-21</t>
+  </si>
+  <si>
+    <t>$ 174.752 CLP 18-03-21</t>
+  </si>
+  <si>
+    <t>23.80 UF 18-03-21</t>
   </si>
 </sst>
 </file>
@@ -488,7 +596,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BFA8BFF-EFDD-4913-9E02-008959E8AF40}">
-  <dimension ref="A1:A105"/>
+  <dimension ref="A1:A165"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
@@ -1024,6 +1132,306 @@
         <v>33</v>
       </c>
     </row>
+    <row r="106">
+      <c r="A106" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Kubernates flujo planes-producto Firefox
</commit_message>
<xml_diff>
--- a/src/test/resources/filepath/Test2.xlsx
+++ b/src/test/resources/filepath/Test2.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="74">
   <si>
     <t>$ 27.323 CLP 17-10-20</t>
   </si>
@@ -250,6 +250,12 @@
   </si>
   <si>
     <t>Propiedad destacada x30;  $587.668;  IVA: $111.657;  Total: $699.325;  25-03-21</t>
+  </si>
+  <si>
+    <t>Propiedad destacada x30;  $587.706;  IVA: $111.664;  Total: $699.370;  26-03-21</t>
+  </si>
+  <si>
+    <t>Plan Escala;  $146.926;  IVA: $27.916;  $174.842;  26-03-21</t>
   </si>
 </sst>
 </file>
@@ -602,7 +608,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BFA8BFF-EFDD-4913-9E02-008959E8AF40}">
-  <dimension ref="A1:A168"/>
+  <dimension ref="A1:A171"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
@@ -1453,6 +1459,21 @@
         <v>71</v>
       </c>
     </row>
+    <row r="169">
+      <c r="A169" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>